<commit_message>
actualizacion del archivo normalizedTags
</commit_message>
<xml_diff>
--- a/resources/npl/normalizedTags.xlsx
+++ b/resources/npl/normalizedTags.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="6330" tabRatio="666"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="6330" tabRatio="666" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="12" r:id="rId1"/>
@@ -3823,6 +3823,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3835,13 +3842,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -5498,8 +5498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5998,7 +5998,7 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6791,7 +6791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -6800,7 +6800,7 @@
     <col min="1" max="1" width="11.42578125" style="5"/>
     <col min="2" max="2" width="12.140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="57" style="4" customWidth="1"/>
     <col min="5" max="5" width="58.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="35.85546875" style="5" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="4"/>
@@ -6826,7 +6826,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -6867,7 +6867,7 @@
       </c>
       <c r="G3" s="182"/>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -6908,7 +6908,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -7056,7 +7056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -7107,7 +7107,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="144" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="96" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="48" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -7524,7 +7524,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -7629,7 +7629,7 @@
       </c>
       <c r="E50" s="182"/>
     </row>
-    <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -7677,7 +7677,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -7725,7 +7725,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7838,7 +7838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K35" sqref="K35:K38"/>
     </sheetView>
   </sheetViews>
@@ -9008,7 +9008,7 @@
         <v>189</v>
       </c>
       <c r="B49" s="68"/>
-      <c r="C49" s="187" t="s">
+      <c r="C49" s="190" t="s">
         <v>168</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -9026,7 +9026,7 @@
         <v>173</v>
       </c>
       <c r="B50" s="68"/>
-      <c r="C50" s="187"/>
+      <c r="C50" s="190"/>
       <c r="E50" s="1" t="s">
         <v>277</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>252</v>
       </c>
       <c r="B51" s="68"/>
-      <c r="C51" s="187"/>
+      <c r="C51" s="190"/>
       <c r="G51" t="s">
         <v>280</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>269</v>
       </c>
       <c r="B52" s="68"/>
-      <c r="C52" s="187"/>
+      <c r="C52" s="190"/>
       <c r="G52" s="85" t="s">
         <v>308</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>254</v>
       </c>
       <c r="B53" s="68"/>
-      <c r="C53" s="187"/>
+      <c r="C53" s="190"/>
       <c r="G53" s="90" t="s">
         <v>294</v>
       </c>
@@ -9097,7 +9097,7 @@
         <v>256</v>
       </c>
       <c r="B54" s="68"/>
-      <c r="C54" s="187"/>
+      <c r="C54" s="190"/>
       <c r="G54" s="90"/>
       <c r="H54" s="84"/>
       <c r="I54" s="84"/>
@@ -9117,7 +9117,7 @@
         <v>42</v>
       </c>
       <c r="B55" s="70"/>
-      <c r="C55" s="188"/>
+      <c r="C55" s="191"/>
       <c r="G55" s="90"/>
       <c r="H55" s="84"/>
       <c r="I55" s="84"/>
@@ -9182,13 +9182,13 @@
         <v>302</v>
       </c>
       <c r="K60" s="81"/>
-      <c r="L60" s="189" t="s">
+      <c r="L60" s="192" t="s">
         <v>306</v>
       </c>
-      <c r="M60" s="189"/>
-      <c r="N60" s="189"/>
-      <c r="O60" s="189"/>
-      <c r="P60" s="189"/>
+      <c r="M60" s="192"/>
+      <c r="N60" s="192"/>
+      <c r="O60" s="192"/>
+      <c r="P60" s="192"/>
     </row>
     <row r="61" spans="1:17" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="81"/>
@@ -9204,13 +9204,13 @@
         <v>303</v>
       </c>
       <c r="L61" s="3"/>
-      <c r="M61" s="189" t="s">
+      <c r="M61" s="192" t="s">
         <v>307</v>
       </c>
-      <c r="N61" s="189"/>
-      <c r="O61" s="189"/>
-      <c r="P61" s="189"/>
-      <c r="Q61" s="189"/>
+      <c r="N61" s="192"/>
+      <c r="O61" s="192"/>
+      <c r="P61" s="192"/>
+      <c r="Q61" s="192"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
@@ -12336,7 +12336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
@@ -12393,18 +12393,18 @@
       <c r="C5" s="78" t="s">
         <v>421</v>
       </c>
-      <c r="F5" s="190" t="s">
+      <c r="F5" s="193" t="s">
         <v>610</v>
       </c>
-      <c r="G5" s="190"/>
-      <c r="H5" s="190"/>
-      <c r="I5" s="190" t="s">
+      <c r="G5" s="193"/>
+      <c r="H5" s="193"/>
+      <c r="I5" s="193" t="s">
         <v>490</v>
       </c>
-      <c r="J5" s="190"/>
-      <c r="K5" s="190"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
+      <c r="J5" s="193"/>
+      <c r="K5" s="193"/>
+      <c r="L5" s="193"/>
+      <c r="M5" s="193"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -13244,1109 +13244,1109 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" style="193" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" style="189" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="189" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="191" t="s">
+      <c r="A2" s="187" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="193">
+      <c r="A3" s="189">
         <v>44165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="189" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="191" t="s">
+      <c r="A5" s="187" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="193">
+      <c r="A6" s="189">
         <v>44164</v>
       </c>
       <c r="B6" s="135"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="193" t="s">
+      <c r="A7" s="189" t="s">
         <v>647</v>
       </c>
       <c r="C7" s="135"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="191" t="s">
+      <c r="A8" s="187" t="s">
         <v>648</v>
       </c>
       <c r="C8" s="135"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="193">
+      <c r="A9" s="189">
         <v>44164</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="193" t="s">
+      <c r="A10" s="189" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="191" t="s">
+      <c r="A11" s="187" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="193">
+      <c r="A12" s="189">
         <v>44164</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="193" t="s">
+      <c r="A13" s="189" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="191" t="s">
+      <c r="A14" s="187" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="193">
+      <c r="A15" s="189">
         <v>44162</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="193" t="s">
+      <c r="A16" s="189" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="191" t="s">
+      <c r="A17" s="187" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="193">
+      <c r="A18" s="189">
         <v>44161</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="193" t="s">
+      <c r="A19" s="189" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="191" t="s">
+      <c r="A20" s="187" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="193">
+      <c r="A21" s="189">
         <v>44161</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="193" t="s">
+      <c r="A22" s="189" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="191" t="s">
+      <c r="A23" s="187" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="193">
+      <c r="A24" s="189">
         <v>44159</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="193" t="s">
+      <c r="A25" s="189" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="191" t="s">
+      <c r="A26" s="187" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="193">
+      <c r="A27" s="189">
         <v>44159</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="193" t="s">
+      <c r="A28" s="189" t="s">
         <v>660</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="191" t="s">
+      <c r="A29" s="187" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="193">
+      <c r="A30" s="189">
         <v>44159</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="193" t="s">
+      <c r="A31" s="189" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="191" t="s">
+      <c r="A32" s="187" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="193">
+      <c r="A33" s="189">
         <v>44159</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="193" t="s">
+      <c r="A34" s="189" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="191" t="s">
+      <c r="A35" s="187" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="193">
+      <c r="A36" s="189">
         <v>44158</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="193" t="s">
+      <c r="A37" s="189" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="191" t="s">
+      <c r="A38" s="187" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="193">
+      <c r="A39" s="189">
         <v>44158</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="193" t="s">
+      <c r="A40" s="189" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="191" t="s">
+      <c r="A41" s="187" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="193">
+      <c r="A42" s="189">
         <v>44157</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="193" t="s">
+      <c r="A43" s="189" t="s">
         <v>669</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="191" t="s">
+      <c r="A44" s="187" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="193">
+      <c r="A45" s="189">
         <v>44156</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="193" t="s">
+      <c r="A46" s="189" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="191" t="s">
+      <c r="A47" s="187" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="193">
+      <c r="A48" s="189">
         <v>44156</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="193" t="s">
+      <c r="A49" s="189" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="191" t="s">
+      <c r="A50" s="187" t="s">
         <v>674</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="193">
+      <c r="A51" s="189">
         <v>44155</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="193" t="s">
+      <c r="A52" s="189" t="s">
         <v>675</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="191" t="s">
+      <c r="A53" s="187" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="193">
+      <c r="A54" s="189">
         <v>44153</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="193" t="s">
+      <c r="A55" s="189" t="s">
         <v>677</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="191" t="s">
+      <c r="A56" s="187" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="193">
+      <c r="A57" s="189">
         <v>44153</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="193" t="s">
+      <c r="A58" s="189" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="191" t="s">
+      <c r="A59" s="187" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="193">
+      <c r="A60" s="189">
         <v>44153</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="193" t="s">
+      <c r="A61" s="189" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="191" t="s">
+      <c r="A62" s="187" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="193">
+      <c r="A63" s="189">
         <v>44153</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="193" t="s">
+      <c r="A64" s="189" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="191" t="s">
+      <c r="A65" s="187" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="193">
+      <c r="A66" s="189">
         <v>44152</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="193" t="s">
+      <c r="A67" s="189" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="193" t="s">
+      <c r="A68" s="189" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="191" t="s">
+      <c r="A69" s="187" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="193">
+      <c r="A70" s="189">
         <v>44151</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="193" t="s">
+      <c r="A71" s="189" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="191" t="s">
+      <c r="A72" s="187" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="193">
+      <c r="A73" s="189">
         <v>44150</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="193" t="s">
+      <c r="A74" s="189" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="191" t="s">
+      <c r="A75" s="187" t="s">
         <v>691</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="193">
+      <c r="A76" s="189">
         <v>44149</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="193" t="s">
+      <c r="A77" s="189" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="191" t="s">
+      <c r="A78" s="187" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="193">
+      <c r="A79" s="189">
         <v>44149</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="193" t="s">
+      <c r="A80" s="189" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="191" t="s">
+      <c r="A81" s="187" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="193">
+      <c r="A82" s="189">
         <v>44148</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="193" t="s">
+      <c r="A83" s="189" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="191" t="s">
+      <c r="A84" s="187" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="193">
+      <c r="A85" s="189">
         <v>44148</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="193" t="s">
+      <c r="A86" s="189" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="191" t="s">
+      <c r="A87" s="187" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="193">
+      <c r="A88" s="189">
         <v>44148</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="193" t="s">
+      <c r="A89" s="189" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="191" t="s">
+      <c r="A90" s="187" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="193">
+      <c r="A91" s="189">
         <v>44148</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="193" t="s">
+      <c r="A92" s="189" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="193" t="s">
+      <c r="A93" s="189" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="191" t="s">
+      <c r="A94" s="187" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="193">
+      <c r="A95" s="189">
         <v>44147</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="193" t="s">
+      <c r="A96" s="189" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="191" t="s">
+      <c r="A97" s="187" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="193">
+      <c r="A98" s="189">
         <v>44147</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="193" t="s">
+      <c r="A99" s="189" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="193" t="s">
+      <c r="A100" s="189" t="s">
         <v>707</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="191" t="s">
+      <c r="A101" s="187" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="193">
+      <c r="A102" s="189">
         <v>44146</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="193" t="s">
+      <c r="A103" s="189" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="191" t="s">
+      <c r="A104" s="187" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="193">
+      <c r="A105" s="189">
         <v>44146</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="193" t="s">
+      <c r="A106" s="189" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="191" t="s">
+      <c r="A107" s="187" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="193">
+      <c r="A108" s="189">
         <v>44146</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="193" t="s">
+      <c r="A109" s="189" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="191" t="s">
+      <c r="A110" s="187" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="193">
+      <c r="A111" s="189">
         <v>44144</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="193" t="s">
+      <c r="A112" s="189" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="191" t="s">
+      <c r="A113" s="187" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="193">
+      <c r="A114" s="189">
         <v>44144</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="193" t="s">
+      <c r="A115" s="189" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="193" t="s">
+      <c r="A116" s="189" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="193" t="s">
+      <c r="A117" s="189" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="191" t="s">
+      <c r="A118" s="187" t="s">
         <v>719</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="193">
+      <c r="A119" s="189">
         <v>44143</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="193" t="s">
+      <c r="A120" s="189" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="191" t="s">
+      <c r="A121" s="187" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="193">
+      <c r="A122" s="189">
         <v>44143</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="193" t="s">
+      <c r="A123" s="189" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="191" t="s">
+      <c r="A124" s="187" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="193">
+      <c r="A125" s="189">
         <v>44141</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="193" t="s">
+      <c r="A126" s="189" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="193" t="s">
+      <c r="A127" s="189" t="s">
         <v>725</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="191" t="s">
+      <c r="A128" s="187" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="193">
+      <c r="A129" s="189">
         <v>44141</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="193" t="s">
+      <c r="A130" s="189" t="s">
         <v>727</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="193" t="s">
+      <c r="A131" s="189" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="191" t="s">
+      <c r="A132" s="187" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="193">
+      <c r="A133" s="189">
         <v>44141</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="193" t="s">
+      <c r="A134" s="189" t="s">
         <v>730</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="191" t="s">
+      <c r="A135" s="187" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="193">
+      <c r="A136" s="189">
         <v>44141</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="193" t="s">
+      <c r="A137" s="189" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="191" t="s">
+      <c r="A138" s="187" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="193">
+      <c r="A139" s="189">
         <v>44140</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="193" t="s">
+      <c r="A140" s="189" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="191" t="s">
+      <c r="A141" s="187" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="193">
+      <c r="A142" s="189">
         <v>44139</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="193" t="s">
+      <c r="A143" s="189" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="191" t="s">
+      <c r="A144" s="187" t="s">
         <v>674</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="193">
+      <c r="A145" s="189">
         <v>44139</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="193" t="s">
+      <c r="A146" s="189" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="191" t="s">
+      <c r="A147" s="187" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="193">
+      <c r="A148" s="189">
         <v>44138</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="193" t="s">
+      <c r="A149" s="189" t="s">
         <v>736</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="191" t="s">
+      <c r="A150" s="187" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="193">
+      <c r="A151" s="189">
         <v>44138</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="193" t="s">
+      <c r="A152" s="189" t="s">
         <v>738</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="191" t="s">
+      <c r="A153" s="187" t="s">
         <v>739</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="193">
+      <c r="A154" s="189">
         <v>44138</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="193" t="s">
+      <c r="A155" s="189" t="s">
         <v>740</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="191" t="s">
+      <c r="A156" s="187" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="193">
+      <c r="A157" s="189">
         <v>44137</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="193" t="s">
+      <c r="A158" s="189" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="191" t="s">
+      <c r="A159" s="187" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="193">
+      <c r="A160" s="189">
         <v>44137</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="193" t="s">
+      <c r="A161" s="189" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="191" t="s">
+      <c r="A162" s="187" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="193">
+      <c r="A163" s="189">
         <v>44137</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="193" t="s">
+      <c r="A164" s="189" t="s">
         <v>744</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="191" t="s">
+      <c r="A165" s="187" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="193">
+      <c r="A166" s="189">
         <v>44136</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="193" t="s">
+      <c r="A167" s="189" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="191" t="s">
+      <c r="A168" s="187" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="193">
+      <c r="A169" s="189">
         <v>44134</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="193" t="s">
+      <c r="A170" s="189" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="191" t="s">
+      <c r="A171" s="187" t="s">
         <v>748</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="193">
+      <c r="A172" s="189">
         <v>44128</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="193" t="s">
+      <c r="A173" s="189" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="191" t="s">
+      <c r="A174" s="187" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="193">
+      <c r="A175" s="189">
         <v>44128</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="193" t="s">
+      <c r="A176" s="189" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="191" t="s">
+      <c r="A177" s="187" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="193">
+      <c r="A178" s="189">
         <v>44128</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="193" t="s">
+      <c r="A179" s="189" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="191" t="s">
+      <c r="A180" s="187" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="193">
+      <c r="A181" s="189">
         <v>44127</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="193" t="s">
+      <c r="A182" s="189" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="191" t="s">
+      <c r="A183" s="187" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="193">
+      <c r="A184" s="189">
         <v>44127</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="193" t="s">
+      <c r="A185" s="189" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="191" t="s">
+      <c r="A186" s="187" t="s">
         <v>757</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="193">
+      <c r="A187" s="189">
         <v>44126</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="193" t="s">
+      <c r="A188" s="189" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="191" t="s">
+      <c r="A189" s="187" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="193">
+      <c r="A190" s="189">
         <v>44126</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="193" t="s">
+      <c r="A191" s="189" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="191" t="s">
+      <c r="A192" s="187" t="s">
         <v>761</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="193">
+      <c r="A193" s="189">
         <v>44125</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="193" t="s">
+      <c r="A194" s="189" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="191" t="s">
+      <c r="A195" s="187" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="193">
+      <c r="A196" s="189">
         <v>44124</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="193" t="s">
+      <c r="A197" s="189" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="191" t="s">
+      <c r="A198" s="187" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="193">
+      <c r="A199" s="189">
         <v>44120</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="193" t="s">
+      <c r="A200" s="189" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="191" t="s">
+      <c r="A201" s="187" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="193">
+      <c r="A202" s="189">
         <v>44118</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="193" t="s">
+      <c r="A203" s="189" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="191" t="s">
+      <c r="A204" s="187" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="193">
+      <c r="A205" s="189">
         <v>44118</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="193" t="s">
+      <c r="A206" s="189" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="191" t="s">
+      <c r="A207" s="187" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="193">
+      <c r="A208" s="189">
         <v>44118</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="193" t="s">
+      <c r="A209" s="189" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="191" t="s">
+      <c r="A210" s="187" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="193">
+      <c r="A211" s="189">
         <v>44118</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="193" t="s">
+      <c r="A212" s="189" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="191" t="s">
+      <c r="A213" s="187" t="s">
         <v>769</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="193">
+      <c r="A214" s="189">
         <v>44118</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" s="193" t="s">
+      <c r="A215" s="189" t="s">
         <v>770</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="191" t="s">
+      <c r="A216" s="187" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="193">
+      <c r="A217" s="189">
         <v>44117</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="193" t="s">
+      <c r="A218" s="189" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="191" t="s">
+      <c r="A219" s="187" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="192">
+      <c r="A220" s="188">
         <v>44117</v>
       </c>
     </row>

</xml_diff>